<commit_message>
Custom formatting fixes and improvements vaadin/spreadsheet#539
Created `CustomDataFormatter` extending `DataFormatter` to add workarounds for custom formatting handling, which is supposed to be handled by POI.

Includes fixes to:

* Locale change
* Literal as format
* Empty formats
* added a workaround for three part custom formats to support Locale based formatting
* added support for string literal formats (eg. '-' for 0)
* negative number with one part format
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet-flow-parent/vaadin-spreadsheet/src/test/resources/test_sheets/custom_format.xlsx
+++ b/vaadin-spreadsheet-flow-parent/vaadin-spreadsheet/src/test/resources/test_sheets/custom_format.xlsx
@@ -1,32 +1,117 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna\Downloads\Tagetik\TAG84\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtzukanov/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="12280"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Supported features" sheetId="1" r:id="rId1"/>
+    <sheet name="Not supported features" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="18">
+  <si>
+    <t>positive</t>
+  </si>
+  <si>
+    <t>negative</t>
+  </si>
+  <si>
+    <t>zero</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>4-part custom formatting</t>
+  </si>
+  <si>
+    <t>3-parts custom formatting</t>
+  </si>
+  <si>
+    <t>2-part custom formatting</t>
+  </si>
+  <si>
+    <t>1-part custom formatting</t>
+  </si>
+  <si>
+    <t>Literals only</t>
+  </si>
+  <si>
+    <t>formatted text</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Containing ; as a string</t>
+  </si>
+  <si>
+    <t>Colors</t>
+  </si>
+  <si>
+    <t>POI cannot handle this case, putting it here for later use if needed</t>
+  </si>
+  <si>
+    <t>Not supported by Spreadsheet</t>
+  </si>
+  <si>
+    <t>Number + literal</t>
+  </si>
+  <si>
+    <t>Could not create "literal";"literal" format, it automatically changes to "literal";"literal";"literal"</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0_);[Red]\(#,##0\);_-* &quot;-&quot;_-;_-@_-"/>
+  <numFmts count="23">
+    <numFmt numFmtId="164" formatCode="#,##0.0\ ;\(#,##0.0\)\ ;&quot;-&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0\ ;\(#,##0.0\)\ ;&quot;-&quot;;@"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0\ ;\(#,##0.0\)\ "/>
+    <numFmt numFmtId="167" formatCode="#,##0.0\ "/>
+    <numFmt numFmtId="168" formatCode="#,##0.0\ ;\(#,##0.0\)\ ;&quot;-&quot;;\&quot;@\&quot;"/>
+    <numFmt numFmtId="169" formatCode="&quot;literal&quot;;&quot;literal&quot;;&quot;literal&quot;;&quot;literal&quot;"/>
+    <numFmt numFmtId="170" formatCode="&quot;literal&quot;;&quot;literal&quot;;&quot;literal&quot;"/>
+    <numFmt numFmtId="171" formatCode="&quot;literal&quot;"/>
+    <numFmt numFmtId="172" formatCode="&quot;literal&quot;;&quot;literal&quot;;&quot;new&quot;"/>
+    <numFmt numFmtId="173" formatCode="[Red]#,##0.0\ "/>
+    <numFmt numFmtId="174" formatCode="[Red]#,##0.0\ ;[Blue]\(#,##0.0\)\ ;[Green]&quot;-&quot;;[Red]\&quot;@\&quot;"/>
+    <numFmt numFmtId="175" formatCode="[Red]#,##0.0\ ;[Blue]\(#,##0.0\)\ ;[Green]&quot;-&quot;"/>
+    <numFmt numFmtId="176" formatCode="[Red]#,##0.0\ ;[Blue]\(#,##0.0\)\ "/>
+    <numFmt numFmtId="177" formatCode=";;"/>
+    <numFmt numFmtId="178" formatCode=";;;"/>
+    <numFmt numFmtId="179" formatCode="&quot;&quot;"/>
+    <numFmt numFmtId="180" formatCode="#,##0.0\ &quot;;test&quot;;\(#,##0.0\)\ &quot;;test&quot;;&quot;-;test&quot;;\&quot;@&quot;;test&quot;\&quot;"/>
+    <numFmt numFmtId="181" formatCode="#,##0.0\ &quot;;test&quot;;\(#,##0.0\)\ &quot;;test&quot;;&quot;-;test&quot;"/>
+    <numFmt numFmtId="182" formatCode="#,##0.0\ &quot;;test&quot;;\(#,##0.0\)\ &quot;;test&quot;"/>
+    <numFmt numFmtId="183" formatCode="#,##0.0\ &quot;;test&quot;"/>
+    <numFmt numFmtId="184" formatCode="#,##0.0\ \+\ &quot;literal&quot;;#,##0.0\ \+\ &quot;literal&quot;;#,##0.0\ \+\ &quot;literal&quot;;@\ \+\ &quot;literal&quot;"/>
+    <numFmt numFmtId="185" formatCode="#,##0.0\ \+\ &quot;literal&quot;;#,##0.0\ \+\ &quot;literal&quot;;#,##0.0\ \+\ &quot;literal&quot;"/>
+    <numFmt numFmtId="186" formatCode="#,##0.0\ \+\ &quot;literal&quot;"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -57,12 +142,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Norm." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -78,7 +190,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-teema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -123,9 +235,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -158,9 +270,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -340,14 +452,584 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="3.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5">
+        <v>5</v>
+      </c>
+      <c r="E1" s="6">
+        <v>5</v>
+      </c>
+      <c r="F1" s="11"/>
+      <c r="G1" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>-5</v>
+      </c>
+      <c r="E2" s="6">
+        <v>-5</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="12">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="E6" s="7">
+        <v>5</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-5</v>
+      </c>
+      <c r="E7" s="7">
+        <v>-5</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="13">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3">
+        <v>5</v>
+      </c>
+      <c r="E11" s="7">
+        <v>5</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>-5</v>
+      </c>
+      <c r="E12" s="7">
+        <v>-5</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="13">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>5</v>
+      </c>
+      <c r="E16" s="8">
+        <v>5</v>
+      </c>
+      <c r="F16" s="11"/>
+      <c r="G16" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4">
+        <v>-5</v>
+      </c>
+      <c r="E17" s="8">
+        <v>-5</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="15">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0</v>
+      </c>
+      <c r="E18" s="8">
+        <v>0</v>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="105" x14ac:dyDescent="0.2">
+      <c r="E22" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="3.5" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="4" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="6"/>
+      <c r="B1" s="16">
+        <v>5</v>
+      </c>
+      <c r="D1" s="19">
+        <v>5</v>
+      </c>
+      <c r="E1" s="11"/>
+      <c r="F1" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="6"/>
+      <c r="B2" s="16">
+        <v>-5</v>
+      </c>
+      <c r="D2" s="19">
+        <v>-5</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="20">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="6"/>
+      <c r="B3" s="16">
+        <v>0</v>
+      </c>
+      <c r="D3" s="19">
+        <v>0</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="6"/>
+      <c r="B4" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="7"/>
+      <c r="B6" s="17">
+        <v>5</v>
+      </c>
+      <c r="D6" s="21">
+        <v>5</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="7"/>
+      <c r="B7" s="17">
+        <v>-5</v>
+      </c>
+      <c r="D7" s="21">
+        <v>-5</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="22">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="7"/>
+      <c r="B8" s="17">
+        <v>0</v>
+      </c>
+      <c r="D8" s="21">
+        <v>0</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="7"/>
+      <c r="B9" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="9"/>
+      <c r="B11" s="17">
+        <v>5</v>
+      </c>
+      <c r="D11" s="23">
+        <v>5</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="9"/>
+      <c r="B12" s="17">
+        <v>-5</v>
+      </c>
+      <c r="D12" s="23">
+        <v>-5</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="24">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="9"/>
+      <c r="B13" s="17">
+        <v>0</v>
+      </c>
+      <c r="D13" s="23">
+        <v>0</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="9"/>
+      <c r="B14" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+      <c r="B16" s="18">
+        <v>5</v>
+      </c>
+      <c r="D16" s="25">
+        <v>5</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
+      <c r="B17" s="18">
+        <v>-5</v>
+      </c>
+      <c r="D17" s="25">
+        <v>-5</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="26">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="8"/>
+      <c r="B18" s="18">
+        <v>0</v>
+      </c>
+      <c r="D18" s="25">
+        <v>0</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="8"/>
+      <c r="B19" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="D22" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>